<commit_message>
Row wise data reading from excel file for multiple columns of test data
</commit_message>
<xml_diff>
--- a/ExcelReader/testData/TestData.xlsx
+++ b/ExcelReader/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{88697896-CF6F-4631-8D9A-19A1DF00B276}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100800_{88EC8409-8BF9-4606-976A-920C7CFB0429}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14150" windowHeight="5590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>T04_Tourism</t>
+  </si>
+  <si>
+    <t>TestCase2</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -450,7 +453,9 @@
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">

</xml_diff>